<commit_message>
adding dei notes from October all-dept meeting
</commit_message>
<xml_diff>
--- a/1290/quiz2_prob1_scores.xlsx
+++ b/1290/quiz2_prob1_scores.xlsx
@@ -1398,8 +1398,8 @@
   </sheetPr>
   <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C208" activeCellId="0" sqref="C208"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F66" activeCellId="0" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1668,7 +1668,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1850,7 +1850,7 @@
         <v>68</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2266,7 +2266,7 @@
         <v>132</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -2292,7 +2292,7 @@
         <v>136</v>
       </c>
       <c r="C68" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -2318,7 +2318,7 @@
         <v>140</v>
       </c>
       <c r="C70" s="2" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -2604,7 +2604,7 @@
         <v>184</v>
       </c>
       <c r="C92" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -2968,7 +2968,7 @@
         <v>240</v>
       </c>
       <c r="C120" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
@@ -3085,7 +3085,7 @@
         <v>258</v>
       </c>
       <c r="C129" s="2" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -3332,7 +3332,7 @@
         <v>296</v>
       </c>
       <c r="C148" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -3956,7 +3956,7 @@
         <v>392</v>
       </c>
       <c r="C196" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>

</xml_diff>